<commit_message>
Implement many more sounds
</commit_message>
<xml_diff>
--- a/AudioAssetList.xlsx
+++ b/AudioAssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Libraries\Projects\UnityStuff\GunCube\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9962B3CE-22E0-4B0C-B7E5-A023593343BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A8D060-621A-49C3-8D9B-80BAF818646B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2685" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>Audio</t>
   </si>
@@ -487,7 +487,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,6 +555,12 @@
       <c r="E4" t="s">
         <v>34</v>
       </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -566,6 +572,12 @@
       <c r="E5" t="s">
         <v>34</v>
       </c>
+      <c r="F5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -594,6 +606,9 @@
       <c r="F7" t="s">
         <v>34</v>
       </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -608,6 +623,9 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -625,6 +643,9 @@
       <c r="F9" t="s">
         <v>34</v>
       </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -639,6 +660,9 @@
       <c r="F10" t="s">
         <v>34</v>
       </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -687,6 +711,15 @@
       <c r="C13" t="s">
         <v>31</v>
       </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -699,6 +732,12 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>